<commit_message>
Processed survey responses thus far.
</commit_message>
<xml_diff>
--- a/analysis/data/survey_responses.xlsx
+++ b/analysis/data/survey_responses.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EC9BCA-AABD-4D21-9188-6C6B30752340}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD200DC-164D-4F22-8B6B-7BA52948A541}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="likert" sheetId="3" r:id="rId2"/>
+    <sheet name="data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="114">
   <si>
     <t>Timestamp</t>
   </si>
@@ -71,9 +72,6 @@
     <t>Chris Ivory rushed 6 times for 4 yards and in Sunday's week 13 loss to the Dolphins.</t>
   </si>
   <si>
-    <t>Latavius Murray chewed up 11 yards on four carries while securing both of his targets for an additional three yards Sunday in Minnesotaâ€™s Week 13 loss to the Patriots.</t>
-  </si>
-  <si>
     <t>Latavius Murray rushed 4 times for 11 yards in the Vikings' week 13 loss to New England.</t>
   </si>
   <si>
@@ -155,9 +153,6 @@
     <t>Anthony Miller of his 2 targets in the Bears' week 13 loss to the Giants.</t>
   </si>
   <si>
-    <t>Sony Michel racked up 63 yards on 17 carries while converting his lone target for a seven-yard pickup Sunday in the Patriotsâ€™ Week 13 win over Minnesota.</t>
-  </si>
-  <si>
     <t>Sony Michel rushed 17 times for 63 yards in the Patriots' week 13 win over the Vikings.</t>
   </si>
   <si>
@@ -341,9 +336,6 @@
     <t>Josh Doctson caught 3 of 5 targets for 51 yards in the Redskins' week 13 loss to the Eagles.</t>
   </si>
   <si>
-    <t>Stefon Diggs absorbed all five of his targets for 49 yards Sunday in Minnesotaâ€™s Week 13 loss to New England.</t>
-  </si>
-  <si>
     <t>Stefon Diggs caught 5 of 5 targets for 49 yards in the Vikings' week 13 loss to New England.</t>
   </si>
   <si>
@@ -357,6 +349,21 @@
   </si>
   <si>
     <t>Jordan Howard rushed 16 times for 76 yards and a touchdown and in the Bears' week 13 loss to the Giants.</t>
+  </si>
+  <si>
+    <t>Stefon Diggs absorbed all five of his targets for 49 yards Sunday in Minnesota's Week 13 loss to New England.</t>
+  </si>
+  <si>
+    <t>Latavius Murray chewed up 11 yards on four carries while securing both of his targets for an additional three yards Sunday in Minnesota's Week 13 loss to the Patriots.</t>
+  </si>
+  <si>
+    <t>Sony Michel racked up 63 yards on 17 carries while converting his lone target for a seven-yard pickup Sunday in the Patriots' Week 13 win over Minnesota.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Avg</t>
   </si>
 </sst>
 </file>
@@ -384,15 +391,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -415,11 +428,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -438,6 +479,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,10 +778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,75 +797,806 @@
     <col min="10" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" s="9" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:23" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>43445.593784722223</v>
+        <v>43445.691608796296</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="C2" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4">
         <v>3</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="I2" s="4">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4">
+        <v>3</v>
+      </c>
+      <c r="L2" s="4">
+        <v>5</v>
+      </c>
+      <c r="M2" s="4">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4">
+        <v>3</v>
+      </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="1:23" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>43445.703148148146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="4">
+        <v>5</v>
+      </c>
+      <c r="J3" s="4">
+        <v>5</v>
+      </c>
+      <c r="K3" s="4">
+        <v>4</v>
+      </c>
+      <c r="L3" s="4">
+        <v>5</v>
+      </c>
+      <c r="M3" s="4">
+        <v>5</v>
+      </c>
+      <c r="N3" s="4">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="1:23" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>43445.743657407409</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5</v>
+      </c>
+      <c r="K4" s="4">
+        <v>5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5</v>
+      </c>
+      <c r="M4" s="4">
+        <v>5</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>43445.691828703704</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4">
+        <v>5</v>
+      </c>
+      <c r="L5" s="4">
+        <v>5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:23" ht="106.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>43445.703252314815</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5</v>
+      </c>
+      <c r="K6" s="4">
+        <v>5</v>
+      </c>
+      <c r="L6" s="4">
+        <v>3</v>
+      </c>
+      <c r="M6" s="4">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:23" ht="106.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>43445.721516203703</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4</v>
+      </c>
+      <c r="K7" s="4">
+        <v>5</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:23" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>43445.738240740742</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>4</v>
+      </c>
+      <c r="K8" s="4">
+        <v>5</v>
+      </c>
+      <c r="L8" s="4">
+        <v>3</v>
+      </c>
+      <c r="M8" s="4">
+        <v>4</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:23" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>43445.755659722221</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="4">
+        <v>5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4">
+        <v>5</v>
+      </c>
+      <c r="M9" s="4">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:23" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>43445.875671296293</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" s="4">
+        <v>4</v>
+      </c>
+      <c r="J10" s="4">
+        <v>5</v>
+      </c>
+      <c r="K10" s="4">
+        <v>5</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5</v>
+      </c>
+      <c r="M10" s="4">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:23" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>43445.803726851853</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>5</v>
+      </c>
+      <c r="L11" s="4">
+        <v>5</v>
+      </c>
+      <c r="M11" s="4">
+        <v>5</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>43445.830543981479</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
+        <v>4</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4</v>
+      </c>
+      <c r="M12" s="4">
+        <v>4</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:23" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>43445.704293981478</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4">
+        <v>4</v>
+      </c>
+      <c r="M13" s="4">
+        <v>3</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>43445.803784722222</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="4">
+        <v>4</v>
+      </c>
+      <c r="J14" s="4">
+        <v>3</v>
+      </c>
+      <c r="K14" s="4">
+        <v>5</v>
+      </c>
+      <c r="L14" s="4">
+        <v>4</v>
+      </c>
+      <c r="M14" s="4">
+        <v>3</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" ht="120" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>43445.693726851852</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="4">
+        <v>5</v>
+      </c>
+      <c r="J15" s="4">
+        <v>3</v>
+      </c>
+      <c r="K15" s="4">
+        <v>5</v>
+      </c>
+      <c r="L15" s="4">
+        <v>5</v>
+      </c>
+      <c r="M15" s="4">
+        <v>4</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>43445.698321759257</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="4">
+        <v>5</v>
+      </c>
+      <c r="J16" s="4">
+        <v>4</v>
+      </c>
+      <c r="K16" s="4">
+        <v>5</v>
+      </c>
+      <c r="L16" s="4">
+        <v>5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>4</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" ht="120" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>43445.699976851851</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="4">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="4">
+        <v>5</v>
+      </c>
+      <c r="J17" s="4">
+        <v>3</v>
+      </c>
+      <c r="K17" s="4">
+        <v>4</v>
+      </c>
+      <c r="L17" s="4">
+        <v>5</v>
+      </c>
+      <c r="M17" s="4">
+        <v>4</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -814,11 +1605,589 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37543E89-DF45-4F68-ACD9-D3AE8B76507B}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+      <c r="H8" s="4">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="G9" s="4">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4">
+        <v>3</v>
+      </c>
+      <c r="I12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>5</v>
+      </c>
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>5</v>
+      </c>
+      <c r="I13" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4</v>
+      </c>
+      <c r="F14" s="4">
+        <v>5</v>
+      </c>
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>5</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>4</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>5</v>
+      </c>
+      <c r="B17" s="10">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10">
+        <v>5</v>
+      </c>
+      <c r="D17" s="10">
+        <v>3</v>
+      </c>
+      <c r="E17" s="10">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10">
+        <v>5</v>
+      </c>
+      <c r="G17" s="10">
+        <v>5</v>
+      </c>
+      <c r="H17" s="10">
+        <v>5</v>
+      </c>
+      <c r="I17" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="12">
+        <f>SUM(A2:A17,D2:D17,G2:G17)</f>
+        <v>204</v>
+      </c>
+      <c r="C21">
+        <f>AVERAGE(A2:A17,D2:D17,G2:G17)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="12">
+        <f>SUM(B2:B17,E2:E17,H2:H17)</f>
+        <v>198</v>
+      </c>
+      <c r="C22">
+        <f>AVERAGE(B2:B17,E2:E17,H2:H17)</f>
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="12">
+        <f>SUM(C2:C17,F2:F17,I2:I17)</f>
+        <v>181</v>
+      </c>
+      <c r="C23">
+        <f>AVERAGE(C2:C17,F2:F17,I2:I17)</f>
+        <v>3.7708333333333335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D9E136-B242-4723-878B-3500877C36AC}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.5546875" defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -841,383 +2210,383 @@
     </row>
     <row r="3" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>10</v>
@@ -1228,7 +2597,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>